<commit_message>
updated OMAP xlsx files
</commit_message>
<xml_diff>
--- a/digital-objects/omap/1-human-lymph-node-ibex/v1.5/raw/omap-1-human-lymph-node-ibex.xlsx
+++ b/digital-objects/omap/1-human-lymph-node-ibex/v1.5/raw/omap-1-human-lymph-node-ibex.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ellenmq/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hrishi/codeBase/CNS/hra-kg/digital-objects/omap/1-human-lymph-node-ibex/v1.5/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D8ABEC-8935-C547-9B9F-E7BD6C55A625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F02E255-A91B-364F-93DB-8F8B8313D11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5740" yWindow="760" windowWidth="34560" windowHeight="20680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="20680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="omap-1-human-lymph-node-ibex" sheetId="1" r:id="rId1"/>
@@ -6016,12 +6016,6 @@
     <t>used to detect AT2R, see above</t>
   </si>
   <si>
-    <t>v1.4</t>
-  </si>
-  <si>
-    <t>June 15, 2024</t>
-  </si>
-  <si>
     <t>target_symbol</t>
   </si>
   <si>
@@ -6035,6 +6029,12 @@
   </si>
   <si>
     <t>https://doi.org/10.48539/HBM656.VQRD.249</t>
+  </si>
+  <si>
+    <t>June 15, 2025</t>
+  </si>
+  <si>
+    <t>v1.5</t>
   </si>
 </sst>
 </file>
@@ -6662,7 +6662,7 @@
   <dimension ref="A1:AR999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -6987,7 +6987,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="1"/>
@@ -7036,7 +7036,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -7085,7 +7085,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1567</v>
+        <v>1571</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="1"/>
@@ -7134,7 +7134,7 @@
         <v>12</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1566</v>
+        <v>1572</v>
       </c>
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
@@ -7189,7 +7189,7 @@
         <v>15</v>
       </c>
       <c r="D11" s="47" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>17</v>
@@ -7219,7 +7219,7 @@
         <v>25</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="O11" s="15" t="s">
         <v>27</v>
@@ -7243,7 +7243,7 @@
         <v>33</v>
       </c>
       <c r="V11" s="15" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
       <c r="W11" s="15" t="s">
         <v>34</v>

</xml_diff>